<commit_message>
feat: add latest data
</commit_message>
<xml_diff>
--- a/data/ST公告/2023-03-09.xlsx
+++ b/data/ST公告/2023-03-09.xlsx
@@ -464,7 +464,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1275,30 +1275,62 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
+          <t>*ST海伦</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>300201</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>*ST海伦:关于收到《行政处罚及市场禁入事先告知书》的公告</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>2023-03-10 00:00:00</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>2023-03-09 21:57:56:000</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>https://data.eastmoney.com/notices/detail/300201/AN202303091584160746.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
           <t>*ST计通</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
+      <c r="B27" t="inlineStr">
         <is>
           <t>300330</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
+      <c r="C27" t="inlineStr">
         <is>
           <t>*ST计通:关于公司股票可能被实施重大违法强制退市的风险提示公告</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>2023-03-10 00:00:00</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>2023-03-10 00:00:00</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
         <is>
           <t>2023-03-09 17:47:36:000</t>
         </is>
       </c>
-      <c r="F26" t="inlineStr">
+      <c r="F27" t="inlineStr">
         <is>
           <t>https://data.eastmoney.com/notices/detail/300330/AN202303091584153631.html</t>
         </is>
@@ -1315,7 +1347,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1553,15 +1585,30 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
+          <t>*ST海伦</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>300201</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
           <t>*ST计通</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="B17" t="inlineStr">
         <is>
           <t>300330</t>
         </is>
       </c>
-      <c r="C16" t="n">
+      <c r="C17" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>